<commit_message>
Minor corrections to BOM SS and step-by-step instructions
Added jumper wires to the BOM. Made minor corrections and
clarifications to step-by-step instructions.
</commit_message>
<xml_diff>
--- a/docs/IV_Swinger2/IV_Swinger2_BOM.xlsx
+++ b/docs/IV_Swinger2/IV_Swinger2_BOM.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-21360" yWindow="0" windowWidth="20280" windowHeight="19640" tabRatio="500"/>
+    <workbookView xWindow="3580" yWindow="0" windowWidth="30640" windowHeight="19760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">BOM!$A$1:$F$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">BOM!$A$1:$F$37</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
   <si>
     <t>Description</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>EFF-cientt 20pcs 15amp Diode Axial Schottky Blocking Diodes for Solar Cells Panel,15SQ045 Schottky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4" Male to Female jumpers (1 blue, 1 red, 1 black) </t>
+  </si>
+  <si>
+    <t>GenBasic 80 Piece Male to Female Solderless Ribbon Dupont Jumper Wires (4 and 8 Inch) for Breadboard Prototyping</t>
   </si>
 </sst>
 </file>
@@ -227,6 +233,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1258,10 +1265,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F97"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1763,7 +1770,7 @@
         <v>10.86</v>
       </c>
       <c r="D26" s="6">
-        <f t="shared" ref="D26:D31" si="3">B26*C26</f>
+        <f t="shared" ref="D26:D32" si="3">B26*C26</f>
         <v>10.86</v>
       </c>
       <c r="E26" s="4" t="s">
@@ -1835,139 +1842,157 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="26">
+    <row r="30" spans="1:6" ht="45">
       <c r="A30" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="5">
+        <v>3</v>
+      </c>
+      <c r="C30" s="20">
+        <f>5.99/80</f>
+        <v>7.4874999999999997E-2</v>
+      </c>
+      <c r="D30" s="6">
+        <f t="shared" si="3"/>
+        <v>0.22462499999999999</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="26">
+      <c r="A31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B31" s="5">
         <v>10</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C31" s="6">
         <f>3.18/50</f>
         <v>6.3600000000000004E-2</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D31" s="6">
         <f t="shared" si="3"/>
         <v>0.63600000000000001</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E31" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F31" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="26">
-      <c r="A31" s="4" t="s">
+    <row r="32" spans="1:6" ht="26">
+      <c r="A32" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B32" s="5">
         <v>10</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C32" s="6">
         <f>5.49/100</f>
         <v>5.4900000000000004E-2</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D32" s="6">
         <f t="shared" si="3"/>
         <v>0.54900000000000004</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F32" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="25"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-    </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="25"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="4" t="s">
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B35" s="5">
         <v>1</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C35" s="6">
         <v>5.2</v>
       </c>
-      <c r="D34" s="6">
-        <f>B34*C34</f>
+      <c r="D35" s="6">
+        <f>B35*C35</f>
         <v>5.2</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E35" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F34" s="7"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="21"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
+      <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="13">
-        <f>SUM(D$3:D35)</f>
-        <v>48.516004166666661</v>
-      </c>
-      <c r="E36" s="11"/>
-      <c r="F36" s="14"/>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="13">
+        <f>SUM(D$3:D36)</f>
+        <v>48.740629166666665</v>
+      </c>
+      <c r="E37" s="11"/>
       <c r="F37" s="14"/>
     </row>
     <row r="38" spans="1:6">
       <c r="F38" s="14"/>
     </row>
-    <row r="39" spans="1:6" ht="16" customHeight="1">
-      <c r="A39" s="16"/>
+    <row r="39" spans="1:6">
       <c r="F39" s="14"/>
     </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="12"/>
+    <row r="40" spans="1:6" ht="16" customHeight="1">
+      <c r="A40" s="16"/>
       <c r="F40" s="14"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="17"/>
+      <c r="A41" s="12"/>
+      <c r="F41" s="14"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="12"/>
-      <c r="F42" s="14"/>
+      <c r="A42" s="17"/>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="12"/>
       <c r="F43" s="14"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="15"/>
+      <c r="A44" s="12"/>
       <c r="F44" s="14"/>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="12"/>
+      <c r="A45" s="15"/>
       <c r="F45" s="14"/>
     </row>
     <row r="46" spans="1:6">
@@ -1975,7 +2000,7 @@
       <c r="F46" s="14"/>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="15"/>
+      <c r="A47" s="12"/>
       <c r="F47" s="14"/>
     </row>
     <row r="48" spans="1:6">
@@ -1987,7 +2012,7 @@
       <c r="F49" s="14"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="12"/>
+      <c r="A50" s="15"/>
       <c r="F50" s="14"/>
     </row>
     <row r="51" spans="1:6">
@@ -1999,22 +2024,22 @@
       <c r="F52" s="14"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="9"/>
+      <c r="A53" s="12"/>
       <c r="F53" s="14"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="12"/>
+      <c r="A54" s="9"/>
       <c r="F54" s="14"/>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="12"/>
       <c r="F55" s="14"/>
     </row>
-    <row r="56" spans="1:6" ht="20" customHeight="1">
+    <row r="56" spans="1:6">
       <c r="A56" s="12"/>
       <c r="F56" s="14"/>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" ht="20" customHeight="1">
       <c r="A57" s="12"/>
       <c r="F57" s="14"/>
     </row>
@@ -2035,15 +2060,15 @@
       <c r="F61" s="14"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="18"/>
+      <c r="A62" s="12"/>
       <c r="F62" s="14"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="15"/>
+      <c r="A63" s="18"/>
       <c r="F63" s="14"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="12"/>
+      <c r="A64" s="15"/>
       <c r="F64" s="14"/>
     </row>
     <row r="65" spans="1:6">
@@ -2056,13 +2081,13 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="12"/>
+      <c r="F67" s="14"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="18"/>
-      <c r="F68" s="14"/>
+      <c r="A68" s="12"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="12"/>
+      <c r="A69" s="18"/>
       <c r="F69" s="14"/>
     </row>
     <row r="70" spans="1:6">
@@ -2090,11 +2115,12 @@
       <c r="F75" s="14"/>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="17"/>
+      <c r="A76" s="12"/>
       <c r="F76" s="14"/>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="17"/>
+      <c r="F77" s="14"/>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="17"/>
@@ -2155,20 +2181,23 @@
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="17"/>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="17"/>
     </row>
   </sheetData>
   <sortState ref="A26:F31">
     <sortCondition descending="1" ref="C26:C31"/>
   </sortState>
   <mergeCells count="8">
-    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
     <mergeCell ref="A25:F25"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="A24:F24"/>
-    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A33:F33"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>